<commit_message>
20250618 - Review day
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202506/Asia Pacific 500.xlsx
+++ b/GUI + Reviews/202506/Asia Pacific 500.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\PM-Indices-IndexOperations\Review Files\Data input files\Factset Data\Calculation file\202506\Preliminary 10.06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\PM-Indices-IndexOperations\Review Files\Data input files\Factset Data\Calculation file\202506\Preliminary 11.06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{491A16CF-F071-46C0-83F6-0FFB12B11EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A538113-CCDD-422D-8E91-6263491F2E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28530" yWindow="-18120" windowWidth="29040" windowHeight="17640" xr2:uid="{466C7369-A381-414B-B54C-43F6FCDFD223}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D989F1D-1FFE-4DB0-8EB0-5D4DE80189F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -887,6 +887,15 @@
     <t>JP3551520004</t>
   </si>
   <si>
+    <t>Dexerials Corp</t>
+  </si>
+  <si>
+    <t>4980-JP</t>
+  </si>
+  <si>
+    <t>JP3548770001</t>
+  </si>
+  <si>
     <t>DEXUS PROPERTY GROUP</t>
   </si>
   <si>
@@ -912,15 +921,6 @@
   </si>
   <si>
     <t>JP3924800000</t>
-  </si>
-  <si>
-    <t>Duality Biotherapeutics, Inc.</t>
-  </si>
-  <si>
-    <t>9606-HK</t>
-  </si>
-  <si>
-    <t>KYG2929M1087</t>
   </si>
   <si>
     <t>DYNO NOBEL LTD</t>
@@ -4891,21 +4891,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4296CCB6-3A5D-421F-A0BE-B56F8AEAABD5}" name="Universe" displayName="Universe" ref="A1:L501" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:L501" xr:uid="{4296CCB6-3A5D-421F-A0BE-B56F8AEAABD5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{29588404-E879-4190-8030-09D2B8E09232}" name="Universe" displayName="Universe" ref="A1:L501" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:L501" xr:uid="{29588404-E879-4190-8030-09D2B8E09232}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{62BA3783-36FF-41C8-BD1A-C00DF2DD3D5A}" name="Rank" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{64093C84-5573-41D7-B9A9-9AE95FA36EC8}" name="Name" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{582EB76C-A428-4C82-93C5-444BBC9F95AA}" name="Ticker" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{03B7B7C9-EDCF-43DB-B7AD-847F89EAA4ED}" name="ISIN" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{26A3839A-56CE-4380-AF91-467E6C87A4EF}" name="Currency (Local)" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{DA5AE7E0-9536-439C-B09F-57371863A704}" name="Price (EUR) " dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{5AB8759F-C7D1-4D10-A8B1-516C61F17C30}" name="NOSH" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{95D2824E-309E-4C3A-86B1-C06898A01D41}" name="Exchange Name (VND)" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{16372C76-0D20-43EC-9432-FA91B805104E}" name="Sec Market Value (EUR)" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{7E8B4112-506F-4D7A-A203-2E914FC9DCCF}" name="20 days aver. turn EUR" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{660F31EB-7FCB-431E-A6C0-043ECA2D9DD2}" name="6 month aver. turnover EUR" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{56BD88BC-D5C2-4CA8-89B0-FAEEB6403D66}" name="3 month average turnover EUR" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{7E1928C6-B17C-459B-A4F2-1E0DDCD4A339}" name="Rank" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{EA17F889-1B86-49FE-9180-9C71EB0C3879}" name="Name" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{CCF5BE3C-878C-499E-8E44-21BE858FD2D0}" name="Ticker" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{FC5FD580-E5F3-4B6F-ACDD-D7AE24E4F8A9}" name="ISIN" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{745DA445-60D2-41D7-AA86-9A237524DC14}" name="Currency (Local)" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{19974CFE-745C-43AB-96C6-DFACE3CBAB94}" name="Price (EUR) " dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{67544BF4-0BE5-4D53-A98D-5C2EE01A57B6}" name="NOSH" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{ECF6B352-AB49-4DDC-B266-B652190D331B}" name="Exchange Name (VND)" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{9C072696-1AD3-412F-8B3A-CAAC3A6D0515}" name="Sec Market Value (EUR)" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{EB6C44FF-8AAA-4E01-AFC4-89DBD947BB56}" name="20 days aver. turn EUR" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{3D7895B8-46E6-49B8-B559-5DE443F0B0A3}" name="6 month aver. turnover EUR" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{C929DDBA-00B5-48C7-BB89-C573E9697356}" name="3 month average turnover EUR" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5227,7 +5227,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BAC1280-8E46-4634-B2DD-014FCA190FE3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674AEDB1-1697-4977-9E36-2A3428742D41}">
   <dimension ref="A1:L501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -8606,28 +8606,28 @@
         <v>285</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F89" s="1">
-        <v>4.0115210000000001</v>
+        <v>11.98443</v>
       </c>
       <c r="G89" s="1">
-        <v>1075565200</v>
+        <v>176418500</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I89" s="1">
-        <v>4314.652</v>
+        <v>2114.2750000000001</v>
       </c>
       <c r="J89" s="1">
-        <v>15539801.5912305</v>
+        <v>16262594.0494009</v>
       </c>
       <c r="K89" s="1">
-        <v>22468047.381267</v>
+        <v>12231029.0935231</v>
       </c>
       <c r="L89" s="1">
-        <v>15479324.7898612</v>
+        <v>12626521.523249</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.2">
@@ -8644,28 +8644,28 @@
         <v>288</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F90" s="1">
-        <v>206.5685</v>
+        <v>4.0115210000000001</v>
       </c>
       <c r="G90" s="1">
-        <v>108425766</v>
+        <v>1075565200</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I90" s="1">
-        <v>22397.35</v>
+        <v>4314.652</v>
       </c>
       <c r="J90" s="1">
-        <v>1079586082.41623</v>
+        <v>15539801.5912305</v>
       </c>
       <c r="K90" s="1">
-        <v>1119520555.0090699</v>
+        <v>22468047.381267</v>
       </c>
       <c r="L90" s="1">
-        <v>1058534374.04807</v>
+        <v>15479324.7898612</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.2">
@@ -8685,25 +8685,25 @@
         <v>15</v>
       </c>
       <c r="F91" s="1">
-        <v>18.382930000000002</v>
+        <v>206.5685</v>
       </c>
       <c r="G91" s="1">
-        <v>142325930</v>
+        <v>108425766</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I91" s="1">
-        <v>2616.3670000000002</v>
+        <v>22397.35</v>
       </c>
       <c r="J91" s="1">
-        <v>40692812.439864904</v>
+        <v>1079586082.41623</v>
       </c>
       <c r="K91" s="1">
-        <v>30167682.307413802</v>
+        <v>1119520555.0090699</v>
       </c>
       <c r="L91" s="1">
-        <v>40532744.204122901</v>
+        <v>1058534374.04807</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.2">
@@ -8720,28 +8720,28 @@
         <v>294</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F92" s="1">
-        <v>24.06653</v>
+        <v>18.382930000000002</v>
       </c>
       <c r="G92" s="1">
-        <v>88036260</v>
+        <v>142325930</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="I92" s="1">
-        <v>2118.7269999999999</v>
+        <v>2616.3670000000002</v>
       </c>
       <c r="J92" s="1">
-        <v>9682544.8182004001</v>
+        <v>40692812.439864904</v>
       </c>
       <c r="K92" s="1">
-        <v>22247093.692638598</v>
+        <v>30167682.307413802</v>
       </c>
       <c r="L92" s="1">
-        <v>22247093.692638598</v>
+        <v>40532744.204122901</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>